<commit_message>
Respuesta final de complejidad de tiempos y recomendacion
</commit_message>
<xml_diff>
--- a/others/Evaluacion de tiempos.xlsx
+++ b/others/Evaluacion de tiempos.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tiempo de mostrar" sheetId="1" r:id="rId1"/>
+    <sheet name="O(n)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Map</t>
   </si>
@@ -54,6 +55,9 @@
   </si>
   <si>
     <t>Mostrar la lista de productos Sorted(ms)</t>
+  </si>
+  <si>
+    <t>Segun el video se concluye que se obtiene un tiempo de O(n*m) dado que es el que mas se tarda, este es un tiempo malo dado que hace mas lento el cpu. Por lo tanto la opcion o la solucion es hacer varios for anexados, de manera de que mediante arrays temporales se trabaje cada for por separado, lo que daria tiempos de k*O(n) de manera que serian practicamente lineales</t>
   </si>
 </sst>
 </file>
@@ -89,14 +93,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -380,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,10 +423,10 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -437,8 +444,8 @@
       <c r="E3" s="1">
         <v>0.32800000000000001</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -456,8 +463,8 @@
       <c r="E4" s="1">
         <v>0.65600000000000003</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -475,32 +482,32 @@
       <c r="E5" s="1">
         <v>0.90800000000000003</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -509,4 +516,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>